<commit_message>
refactor for import order with product
</commit_message>
<xml_diff>
--- a/storage/sample_excel/orders_sample_data.xlsx
+++ b/storage/sample_excel/orders_sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\qlbh\storage\sample_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07264438-ED1C-4835-AAB5-571B5DB52063}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE56E669-5783-440E-8130-228AB6BC979A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Customer</t>
   </si>
@@ -28,27 +28,178 @@
     <t>Order Date</t>
   </si>
   <si>
-    <t>63a1852c648654fb980041c4</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>25/11/1999</t>
-  </si>
-  <si>
-    <t>25/11/1399</t>
+    <t>banh  bao;12000;23</t>
+  </si>
+  <si>
+    <t>banh  bao 2;12000;23</t>
+  </si>
+  <si>
+    <t>banh  bao 3;23000;10</t>
+  </si>
+  <si>
+    <t>thung rac;12000;23</t>
+  </si>
+  <si>
+    <t>thung rac;50000;12</t>
+  </si>
+  <si>
+    <t>Customer 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">From </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> column to the right (end: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> columm),</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> each cell is the product data in the order via format </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;name&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;price&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&lt;quantity&gt; </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,8 +222,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,46 +543,56 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>44879</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44879</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>